<commit_message>
début d'ajout de la méthode avec le point deja présent et petit refactoring de classes.py et main.py
</commit_message>
<xml_diff>
--- a/ListPoint.xlsx
+++ b/ListPoint.xlsx
@@ -262,7 +262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C421"/>
+  <dimension ref="A1:C793"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
@@ -4352,553 +4352,4645 @@
       </c>
     </row>
     <row r="372">
-      <c r="A372" t="n">
+      <c r="A372" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B372" t="n">
+      <c r="B372" s="0" t="n">
         <v>643</v>
       </c>
-      <c r="C372" t="n">
+      <c r="C372" s="0" t="n">
         <v>424</v>
       </c>
     </row>
     <row r="373">
-      <c r="A373" t="n">
+      <c r="A373" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B373" t="n">
+      <c r="B373" s="0" t="n">
         <v>1165</v>
       </c>
-      <c r="C373" t="n">
+      <c r="C373" s="0" t="n">
         <v>446</v>
       </c>
     </row>
     <row r="374">
-      <c r="A374" t="n">
+      <c r="A374" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B374" t="n">
+      <c r="B374" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C374" t="n">
+      <c r="C374" s="0" t="n">
         <v>680</v>
       </c>
     </row>
     <row r="375">
-      <c r="A375" t="n">
+      <c r="A375" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B375" t="n">
+      <c r="B375" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="C375" t="n">
+      <c r="C375" s="0" t="n">
         <v>161</v>
       </c>
     </row>
     <row r="376">
-      <c r="A376" t="n">
+      <c r="A376" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B376" t="n">
+      <c r="B376" s="0" t="n">
         <v>989</v>
       </c>
-      <c r="C376" t="n">
+      <c r="C376" s="0" t="n">
         <v>440</v>
       </c>
     </row>
     <row r="377">
-      <c r="A377" t="n">
+      <c r="A377" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B377" t="n">
+      <c r="B377" s="0" t="n">
         <v>957</v>
       </c>
-      <c r="C377" t="n">
+      <c r="C377" s="0" t="n">
         <v>84</v>
       </c>
     </row>
     <row r="378">
-      <c r="A378" t="n">
+      <c r="A378" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B378" t="n">
+      <c r="B378" s="0" t="n">
         <v>441</v>
       </c>
-      <c r="C378" t="n">
+      <c r="C378" s="0" t="n">
         <v>157</v>
       </c>
     </row>
     <row r="379">
-      <c r="A379" t="n">
+      <c r="A379" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B379" t="n">
+      <c r="B379" s="0" t="n">
         <v>801</v>
       </c>
-      <c r="C379" t="n">
+      <c r="C379" s="0" t="n">
         <v>128</v>
       </c>
     </row>
     <row r="380">
-      <c r="A380" t="n">
+      <c r="A380" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B380" t="n">
+      <c r="B380" s="0" t="n">
         <v>215</v>
       </c>
-      <c r="C380" t="n">
+      <c r="C380" s="0" t="n">
         <v>360</v>
       </c>
     </row>
     <row r="381">
-      <c r="A381" t="n">
+      <c r="A381" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B381" t="n">
+      <c r="B381" s="0" t="n">
         <v>737</v>
       </c>
-      <c r="C381" t="n">
+      <c r="C381" s="0" t="n">
         <v>449</v>
       </c>
     </row>
     <row r="382">
-      <c r="A382" t="n">
+      <c r="A382" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B382" t="n">
+      <c r="B382" s="0" t="n">
         <v>261</v>
       </c>
-      <c r="C382" t="n">
+      <c r="C382" s="0" t="n">
         <v>354</v>
       </c>
     </row>
     <row r="383">
-      <c r="A383" t="n">
+      <c r="A383" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B383" t="n">
+      <c r="B383" s="0" t="n">
         <v>479</v>
       </c>
-      <c r="C383" t="n">
+      <c r="C383" s="0" t="n">
         <v>433</v>
       </c>
     </row>
     <row r="384">
-      <c r="A384" t="n">
+      <c r="A384" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B384" t="n">
+      <c r="B384" s="0" t="n">
         <v>1180</v>
       </c>
-      <c r="C384" t="n">
+      <c r="C384" s="0" t="n">
         <v>494</v>
       </c>
     </row>
     <row r="385">
-      <c r="A385" t="n">
+      <c r="A385" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B385" t="n">
+      <c r="B385" s="0" t="n">
         <v>1198</v>
       </c>
-      <c r="C385" t="n">
+      <c r="C385" s="0" t="n">
         <v>77</v>
       </c>
     </row>
     <row r="386">
-      <c r="A386" t="n">
+      <c r="A386" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B386" t="n">
+      <c r="B386" s="0" t="n">
         <v>619</v>
       </c>
-      <c r="C386" t="n">
+      <c r="C386" s="0" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="387">
-      <c r="A387" t="n">
+      <c r="A387" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B387" t="n">
+      <c r="B387" s="0" t="n">
         <v>691</v>
       </c>
-      <c r="C387" t="n">
+      <c r="C387" s="0" t="n">
         <v>257</v>
       </c>
     </row>
     <row r="388">
-      <c r="A388" t="n">
+      <c r="A388" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B388" t="n">
+      <c r="B388" s="0" t="n">
         <v>1186</v>
       </c>
-      <c r="C388" t="n">
+      <c r="C388" s="0" t="n">
         <v>796</v>
       </c>
     </row>
     <row r="389">
-      <c r="A389" t="n">
+      <c r="A389" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B389" t="n">
+      <c r="B389" s="0" t="n">
         <v>1057</v>
       </c>
-      <c r="C389" t="n">
+      <c r="C389" s="0" t="n">
         <v>825</v>
       </c>
     </row>
     <row r="390">
-      <c r="A390" t="n">
+      <c r="A390" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B390" t="n">
+      <c r="B390" s="0" t="n">
         <v>288</v>
       </c>
-      <c r="C390" t="n">
+      <c r="C390" s="0" t="n">
         <v>392</v>
       </c>
     </row>
     <row r="391">
-      <c r="A391" t="n">
+      <c r="A391" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B391" t="n">
+      <c r="B391" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C391" t="n">
+      <c r="C391" s="0" t="n">
         <v>165</v>
       </c>
     </row>
     <row r="392">
-      <c r="A392" t="n">
+      <c r="A392" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B392" t="n">
+      <c r="B392" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="C392" t="n">
+      <c r="C392" s="0" t="n">
         <v>442</v>
       </c>
     </row>
     <row r="393">
-      <c r="A393" t="n">
+      <c r="A393" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B393" t="n">
+      <c r="B393" s="0" t="n">
         <v>657</v>
       </c>
-      <c r="C393" t="n">
+      <c r="C393" s="0" t="n">
         <v>208</v>
       </c>
     </row>
     <row r="394">
-      <c r="A394" t="n">
+      <c r="A394" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B394" t="n">
+      <c r="B394" s="0" t="n">
         <v>486</v>
       </c>
-      <c r="C394" t="n">
+      <c r="C394" s="0" t="n">
         <v>153</v>
       </c>
     </row>
     <row r="395">
-      <c r="A395" t="n">
+      <c r="A395" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B395" t="n">
+      <c r="B395" s="0" t="n">
         <v>697</v>
       </c>
-      <c r="C395" t="n">
+      <c r="C395" s="0" t="n">
         <v>597</v>
       </c>
     </row>
     <row r="396">
-      <c r="A396" t="n">
+      <c r="A396" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B396" t="n">
+      <c r="B396" s="0" t="n">
         <v>439</v>
       </c>
-      <c r="C396" t="n">
+      <c r="C396" s="0" t="n">
         <v>417</v>
       </c>
     </row>
     <row r="397">
-      <c r="A397" t="n">
+      <c r="A397" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B397" t="n">
+      <c r="B397" s="0" t="n">
         <v>879</v>
       </c>
-      <c r="C397" t="n">
+      <c r="C397" s="0" t="n">
         <v>859</v>
       </c>
     </row>
     <row r="398">
-      <c r="A398" t="n">
+      <c r="A398" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B398" t="n">
+      <c r="B398" s="0" t="n">
         <v>416</v>
       </c>
-      <c r="C398" t="n">
+      <c r="C398" s="0" t="n">
         <v>247</v>
       </c>
     </row>
     <row r="399">
-      <c r="A399" t="n">
+      <c r="A399" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B399" t="n">
+      <c r="B399" s="0" t="n">
         <v>1083</v>
       </c>
-      <c r="C399" t="n">
+      <c r="C399" s="0" t="n">
         <v>236</v>
       </c>
     </row>
     <row r="400">
-      <c r="A400" t="n">
+      <c r="A400" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B400" t="n">
+      <c r="B400" s="0" t="n">
         <v>939</v>
       </c>
-      <c r="C400" t="n">
+      <c r="C400" s="0" t="n">
         <v>375</v>
       </c>
     </row>
     <row r="401">
-      <c r="A401" t="n">
+      <c r="A401" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B401" t="n">
+      <c r="B401" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="C401" t="n">
+      <c r="C401" s="0" t="n">
         <v>188</v>
       </c>
     </row>
     <row r="402">
-      <c r="A402" t="n">
+      <c r="A402" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B402" t="n">
+      <c r="B402" s="0" t="n">
         <v>1112</v>
       </c>
-      <c r="C402" t="n">
+      <c r="C402" s="0" t="n">
         <v>239</v>
       </c>
     </row>
     <row r="403">
-      <c r="A403" t="n">
+      <c r="A403" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B403" t="n">
+      <c r="B403" s="0" t="n">
         <v>165</v>
       </c>
-      <c r="C403" t="n">
+      <c r="C403" s="0" t="n">
         <v>890</v>
       </c>
     </row>
     <row r="404">
-      <c r="A404" t="n">
+      <c r="A404" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B404" t="n">
+      <c r="B404" s="0" t="n">
         <v>809</v>
       </c>
-      <c r="C404" t="n">
+      <c r="C404" s="0" t="n">
         <v>467</v>
       </c>
     </row>
     <row r="405">
-      <c r="A405" t="n">
+      <c r="A405" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B405" t="n">
+      <c r="B405" s="0" t="n">
         <v>1192</v>
       </c>
-      <c r="C405" t="n">
+      <c r="C405" s="0" t="n">
         <v>591</v>
       </c>
     </row>
     <row r="406">
-      <c r="A406" t="n">
+      <c r="A406" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B406" t="n">
+      <c r="B406" s="0" t="n">
         <v>879</v>
       </c>
-      <c r="C406" t="n">
+      <c r="C406" s="0" t="n">
         <v>425</v>
       </c>
     </row>
     <row r="407">
-      <c r="A407" t="n">
+      <c r="A407" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B407" t="n">
+      <c r="B407" s="0" t="n">
         <v>913</v>
       </c>
-      <c r="C407" t="n">
+      <c r="C407" s="0" t="n">
         <v>331</v>
       </c>
     </row>
     <row r="408">
-      <c r="A408" t="n">
+      <c r="A408" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B408" t="n">
+      <c r="B408" s="0" t="n">
         <v>1070</v>
       </c>
-      <c r="C408" t="n">
+      <c r="C408" s="0" t="n">
         <v>721</v>
       </c>
     </row>
     <row r="409">
-      <c r="A409" t="n">
+      <c r="A409" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B409" t="n">
+      <c r="B409" s="0" t="n">
         <v>1015</v>
       </c>
-      <c r="C409" t="n">
+      <c r="C409" s="0" t="n">
         <v>780</v>
       </c>
     </row>
     <row r="410">
-      <c r="A410" t="n">
+      <c r="A410" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B410" t="n">
+      <c r="B410" s="0" t="n">
         <v>334</v>
       </c>
-      <c r="C410" t="n">
+      <c r="C410" s="0" t="n">
         <v>692</v>
       </c>
     </row>
     <row r="411">
-      <c r="A411" t="n">
+      <c r="A411" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B411" t="n">
+      <c r="B411" s="0" t="n">
         <v>633</v>
       </c>
-      <c r="C411" t="n">
+      <c r="C411" s="0" t="n">
         <v>92</v>
       </c>
     </row>
     <row r="412">
-      <c r="A412" t="n">
+      <c r="A412" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B412" t="n">
+      <c r="B412" s="0" t="n">
         <v>1136</v>
       </c>
-      <c r="C412" t="n">
+      <c r="C412" s="0" t="n">
         <v>710</v>
       </c>
     </row>
     <row r="413">
-      <c r="A413" t="n">
+      <c r="A413" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B413" t="n">
+      <c r="B413" s="0" t="n">
         <v>210</v>
       </c>
-      <c r="C413" t="n">
+      <c r="C413" s="0" t="n">
         <v>666</v>
       </c>
     </row>
     <row r="414">
-      <c r="A414" t="n">
+      <c r="A414" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B414" t="n">
+      <c r="B414" s="0" t="n">
         <v>583</v>
       </c>
-      <c r="C414" t="n">
+      <c r="C414" s="0" t="n">
         <v>388</v>
       </c>
     </row>
     <row r="415">
-      <c r="A415" t="n">
+      <c r="A415" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B415" t="n">
+      <c r="B415" s="0" t="n">
         <v>686</v>
       </c>
-      <c r="C415" t="n">
+      <c r="C415" s="0" t="n">
         <v>670</v>
       </c>
     </row>
     <row r="416">
-      <c r="A416" t="n">
+      <c r="A416" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B416" t="n">
+      <c r="B416" s="0" t="n">
         <v>621</v>
       </c>
-      <c r="C416" t="n">
+      <c r="C416" s="0" t="n">
         <v>457</v>
       </c>
     </row>
     <row r="417">
-      <c r="A417" t="n">
+      <c r="A417" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B417" t="n">
+      <c r="B417" s="0" t="n">
         <v>696</v>
       </c>
-      <c r="C417" t="n">
+      <c r="C417" s="0" t="n">
         <v>216</v>
       </c>
     </row>
     <row r="418">
-      <c r="A418" t="n">
+      <c r="A418" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B418" t="n">
+      <c r="B418" s="0" t="n">
         <v>834</v>
       </c>
-      <c r="C418" t="n">
+      <c r="C418" s="0" t="n">
         <v>876</v>
       </c>
     </row>
     <row r="419">
-      <c r="A419" t="n">
+      <c r="A419" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B419" t="n">
+      <c r="B419" s="0" t="n">
         <v>905</v>
       </c>
-      <c r="C419" t="n">
+      <c r="C419" s="0" t="n">
         <v>126</v>
       </c>
     </row>
     <row r="420">
-      <c r="A420" t="n">
+      <c r="A420" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B420" t="n">
+      <c r="B420" s="0" t="n">
         <v>417</v>
       </c>
-      <c r="C420" t="n">
+      <c r="C420" s="0" t="n">
         <v>750</v>
       </c>
     </row>
     <row r="421">
-      <c r="A421" t="n">
+      <c r="A421" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B421" t="n">
+      <c r="B421" s="0" t="n">
         <v>1099</v>
       </c>
-      <c r="C421" t="n">
+      <c r="C421" s="0" t="n">
         <v>245</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B422" s="0" t="n">
+        <v>885</v>
+      </c>
+      <c r="C422" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B423" s="0" t="n">
+        <v>419</v>
+      </c>
+      <c r="C423" s="0" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B424" s="0" t="n">
+        <v>482</v>
+      </c>
+      <c r="C424" s="0" t="n">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B425" s="0" t="n">
+        <v>466</v>
+      </c>
+      <c r="C425" s="0" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B426" s="0" t="n">
+        <v>297</v>
+      </c>
+      <c r="C426" s="0" t="n">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B427" s="0" t="n">
+        <v>482</v>
+      </c>
+      <c r="C427" s="0" t="n">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B428" s="0" t="n">
+        <v>278</v>
+      </c>
+      <c r="C428" s="0" t="n">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B429" s="0" t="n">
+        <v>1102</v>
+      </c>
+      <c r="C429" s="0" t="n">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B430" s="0" t="n">
+        <v>959</v>
+      </c>
+      <c r="C430" s="0" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B431" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="C431" s="0" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B432" s="0" t="n">
+        <v>1142</v>
+      </c>
+      <c r="C432" s="0" t="n">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B433" s="0" t="n">
+        <v>531</v>
+      </c>
+      <c r="C433" s="0" t="n">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B434" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C434" s="0" t="n">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B435" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="C435" s="0" t="n">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B436" s="0" t="n">
+        <v>852</v>
+      </c>
+      <c r="C436" s="0" t="n">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B437" s="0" t="n">
+        <v>974</v>
+      </c>
+      <c r="C437" s="0" t="n">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B438" s="0" t="n">
+        <v>738</v>
+      </c>
+      <c r="C438" s="0" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B439" s="0" t="n">
+        <v>521</v>
+      </c>
+      <c r="C439" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B440" s="0" t="n">
+        <v>943</v>
+      </c>
+      <c r="C440" s="0" t="n">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B441" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="C441" s="0" t="n">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B442" s="0" t="n">
+        <v>268</v>
+      </c>
+      <c r="C442" s="0" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B443" s="0" t="n">
+        <v>792</v>
+      </c>
+      <c r="C443" s="0" t="n">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B444" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="C444" s="0" t="n">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B445" s="0" t="n">
+        <v>941</v>
+      </c>
+      <c r="C445" s="0" t="n">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B446" s="0" t="n">
+        <v>1190</v>
+      </c>
+      <c r="C446" s="0" t="n">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B447" s="0" t="n">
+        <v>1147</v>
+      </c>
+      <c r="C447" s="0" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B448" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="C448" s="0" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B449" s="0" t="n">
+        <v>822</v>
+      </c>
+      <c r="C449" s="0" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B450" s="0" t="n">
+        <v>664</v>
+      </c>
+      <c r="C450" s="0" t="n">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B451" s="0" t="n">
+        <v>791</v>
+      </c>
+      <c r="C451" s="0" t="n">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B452" s="0" t="n">
+        <v>1077</v>
+      </c>
+      <c r="C452" s="0" t="n">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B453" s="0" t="n">
+        <v>431</v>
+      </c>
+      <c r="C453" s="0" t="n">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B454" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="C454" s="0" t="n">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B455" s="0" t="n">
+        <v>778</v>
+      </c>
+      <c r="C455" s="0" t="n">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B456" s="0" t="n">
+        <v>1040</v>
+      </c>
+      <c r="C456" s="0" t="n">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B457" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="C457" s="0" t="n">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B458" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C458" s="0" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B459" s="0" t="n">
+        <v>950</v>
+      </c>
+      <c r="C459" s="0" t="n">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B460" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="C460" s="0" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B461" s="0" t="n">
+        <v>707</v>
+      </c>
+      <c r="C461" s="0" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B462" s="0" t="n">
+        <v>909</v>
+      </c>
+      <c r="C462" s="0" t="n">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B463" s="0" t="n">
+        <v>736</v>
+      </c>
+      <c r="C463" s="0" t="n">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B464" s="0" t="n">
+        <v>1107</v>
+      </c>
+      <c r="C464" s="0" t="n">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B465" s="0" t="n">
+        <v>1141</v>
+      </c>
+      <c r="C465" s="0" t="n">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B466" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C466" s="0" t="n">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B467" s="0" t="n">
+        <v>347</v>
+      </c>
+      <c r="C467" s="0" t="n">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B468" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="C468" s="0" t="n">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B469" s="0" t="n">
+        <v>923</v>
+      </c>
+      <c r="C469" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B470" s="0" t="n">
+        <v>1198</v>
+      </c>
+      <c r="C470" s="0" t="n">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B471" s="0" t="n">
+        <v>743</v>
+      </c>
+      <c r="C471" s="0" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B472" s="0" t="n">
+        <v>720</v>
+      </c>
+      <c r="C472" s="0" t="n">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B473" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="C473" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B474" s="0" t="n">
+        <v>716</v>
+      </c>
+      <c r="C474" s="0" t="n">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B475" s="0" t="n">
+        <v>802</v>
+      </c>
+      <c r="C475" s="0" t="n">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B476" s="0" t="n">
+        <v>391</v>
+      </c>
+      <c r="C476" s="0" t="n">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B477" s="0" t="n">
+        <v>902</v>
+      </c>
+      <c r="C477" s="0" t="n">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B478" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="C478" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B479" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C479" s="0" t="n">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B480" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C480" s="0" t="n">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B481" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="C481" s="0" t="n">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B482" s="0" t="n">
+        <v>382</v>
+      </c>
+      <c r="C482" s="0" t="n">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B483" s="0" t="n">
+        <v>675</v>
+      </c>
+      <c r="C483" s="0" t="n">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B484" s="0" t="n">
+        <v>983</v>
+      </c>
+      <c r="C484" s="0" t="n">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B485" s="0" t="n">
+        <v>1087</v>
+      </c>
+      <c r="C485" s="0" t="n">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B486" s="0" t="n">
+        <v>278</v>
+      </c>
+      <c r="C486" s="0" t="n">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B487" s="0" t="n">
+        <v>1090</v>
+      </c>
+      <c r="C487" s="0" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B488" s="0" t="n">
+        <v>667</v>
+      </c>
+      <c r="C488" s="0" t="n">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B489" s="0" t="n">
+        <v>734</v>
+      </c>
+      <c r="C489" s="0" t="n">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B490" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="C490" s="0" t="n">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B491" s="0" t="n">
+        <v>907</v>
+      </c>
+      <c r="C491" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B492" s="0" t="n">
+        <v>1185</v>
+      </c>
+      <c r="C492" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B493" s="0" t="n">
+        <v>978</v>
+      </c>
+      <c r="C493" s="0" t="n">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B494" s="0" t="n">
+        <v>846</v>
+      </c>
+      <c r="C494" s="0" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B495" s="0" t="n">
+        <v>386</v>
+      </c>
+      <c r="C495" s="0" t="n">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B496" s="0" t="n">
+        <v>510</v>
+      </c>
+      <c r="C496" s="0" t="n">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B497" s="0" t="n">
+        <v>1067</v>
+      </c>
+      <c r="C497" s="0" t="n">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B498" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="C498" s="0" t="n">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B499" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C499" s="0" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B500" s="0" t="n">
+        <v>998</v>
+      </c>
+      <c r="C500" s="0" t="n">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B501" s="0" t="n">
+        <v>468</v>
+      </c>
+      <c r="C501" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B502" s="0" t="n">
+        <v>889</v>
+      </c>
+      <c r="C502" s="0" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B503" s="0" t="n">
+        <v>618</v>
+      </c>
+      <c r="C503" s="0" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B504" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C504" s="0" t="n">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="B505" s="0" t="n">
+        <v>392</v>
+      </c>
+      <c r="C505" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B506" s="0" t="n">
+        <v>274</v>
+      </c>
+      <c r="C506" s="0" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B507" s="0" t="n">
+        <v>228</v>
+      </c>
+      <c r="C507" s="0" t="n">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B508" s="0" t="n">
+        <v>948</v>
+      </c>
+      <c r="C508" s="0" t="n">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B509" s="0" t="n">
+        <v>792</v>
+      </c>
+      <c r="C509" s="0" t="n">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B510" s="0" t="n">
+        <v>1113</v>
+      </c>
+      <c r="C510" s="0" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B511" s="0" t="n">
+        <v>967</v>
+      </c>
+      <c r="C511" s="0" t="n">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B512" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C512" s="0" t="n">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B513" s="0" t="n">
+        <v>906</v>
+      </c>
+      <c r="C513" s="0" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B514" s="0" t="n">
+        <v>767</v>
+      </c>
+      <c r="C514" s="0" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B515" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="C515" s="0" t="n">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B516" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="C516" s="0" t="n">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B517" s="0" t="n">
+        <v>531</v>
+      </c>
+      <c r="C517" s="0" t="n">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B518" s="0" t="n">
+        <v>638</v>
+      </c>
+      <c r="C518" s="0" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B519" s="0" t="n">
+        <v>767</v>
+      </c>
+      <c r="C519" s="0" t="n">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B520" s="0" t="n">
+        <v>708</v>
+      </c>
+      <c r="C520" s="0" t="n">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B521" s="0" t="n">
+        <v>769</v>
+      </c>
+      <c r="C521" s="0" t="n">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B522" s="0" t="n">
+        <v>956</v>
+      </c>
+      <c r="C522" s="0" t="n">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B523" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="C523" s="0" t="n">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B524" s="0" t="n">
+        <v>1048</v>
+      </c>
+      <c r="C524" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B525" s="0" t="n">
+        <v>650</v>
+      </c>
+      <c r="C525" s="0" t="n">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B526" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="C526" s="0" t="n">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B527" s="0" t="n">
+        <v>1170</v>
+      </c>
+      <c r="C527" s="0" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="B528" s="0" t="n">
+        <v>782</v>
+      </c>
+      <c r="C528" s="0" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="B529" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="C529" s="0" t="n">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B530" s="0" t="n">
+        <v>660</v>
+      </c>
+      <c r="C530" s="0" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B531" s="0" t="n">
+        <v>892</v>
+      </c>
+      <c r="C531" s="0" t="n">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B532" s="0" t="n">
+        <v>1057</v>
+      </c>
+      <c r="C532" s="0" t="n">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B533" s="0" t="n">
+        <v>1052</v>
+      </c>
+      <c r="C533" s="0" t="n">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B534" s="0" t="n">
+        <v>593</v>
+      </c>
+      <c r="C534" s="0" t="n">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B535" s="0" t="n">
+        <v>611</v>
+      </c>
+      <c r="C535" s="0" t="n">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B536" s="0" t="n">
+        <v>452</v>
+      </c>
+      <c r="C536" s="0" t="n">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B537" s="0" t="n">
+        <v>703</v>
+      </c>
+      <c r="C537" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B538" s="0" t="n">
+        <v>724</v>
+      </c>
+      <c r="C538" s="0" t="n">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="B539" s="0" t="n">
+        <v>1017</v>
+      </c>
+      <c r="C539" s="0" t="n">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B540" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="C540" s="0" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="B541" s="0" t="n">
+        <v>1155</v>
+      </c>
+      <c r="C541" s="0" t="n">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="B542" s="0" t="n">
+        <v>283</v>
+      </c>
+      <c r="C542" s="0" t="n">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="B543" s="0" t="n">
+        <v>1156</v>
+      </c>
+      <c r="C543" s="0" t="n">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="B544" s="0" t="n">
+        <v>985</v>
+      </c>
+      <c r="C544" s="0" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="B545" s="0" t="n">
+        <v>661</v>
+      </c>
+      <c r="C545" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B546" s="0" t="n">
+        <v>383</v>
+      </c>
+      <c r="C546" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="B547" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="C547" s="0" t="n">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="B548" s="0" t="n">
+        <v>569</v>
+      </c>
+      <c r="C548" s="0" t="n">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="B549" s="0" t="n">
+        <v>1051</v>
+      </c>
+      <c r="C549" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="B550" s="0" t="n">
+        <v>1040</v>
+      </c>
+      <c r="C550" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B551" s="0" t="n">
+        <v>782</v>
+      </c>
+      <c r="C551" s="0" t="n">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B552" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C552" s="0" t="n">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B553" s="0" t="n">
+        <v>631</v>
+      </c>
+      <c r="C553" s="0" t="n">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B554" s="0" t="n">
+        <v>381</v>
+      </c>
+      <c r="C554" s="0" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B555" s="0" t="n">
+        <v>573</v>
+      </c>
+      <c r="C555" s="0" t="n">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B556" s="0" t="n">
+        <v>412</v>
+      </c>
+      <c r="C556" s="0" t="n">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B557" s="0" t="n">
+        <v>913</v>
+      </c>
+      <c r="C557" s="0" t="n">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B558" s="0" t="n">
+        <v>498</v>
+      </c>
+      <c r="C558" s="0" t="n">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B559" s="0" t="n">
+        <v>942</v>
+      </c>
+      <c r="C559" s="0" t="n">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B560" s="0" t="n">
+        <v>368</v>
+      </c>
+      <c r="C560" s="0" t="n">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B561" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="C561" s="0" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B562" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="C562" s="0" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B563" s="0" t="n">
+        <v>248</v>
+      </c>
+      <c r="C563" s="0" t="n">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B564" s="0" t="n">
+        <v>463</v>
+      </c>
+      <c r="C564" s="0" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B565" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="C565" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B566" s="0" t="n">
+        <v>1135</v>
+      </c>
+      <c r="C566" s="0" t="n">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B567" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="C567" s="0" t="n">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B568" s="0" t="n">
+        <v>339</v>
+      </c>
+      <c r="C568" s="0" t="n">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B569" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C569" s="0" t="n">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B570" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="C570" s="0" t="n">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B571" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="C571" s="0" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B572" s="0" t="n">
+        <v>1031</v>
+      </c>
+      <c r="C572" s="0" t="n">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B573" s="0" t="n">
+        <v>793</v>
+      </c>
+      <c r="C573" s="0" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B574" s="0" t="n">
+        <v>690</v>
+      </c>
+      <c r="C574" s="0" t="n">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B575" s="0" t="n">
+        <v>775</v>
+      </c>
+      <c r="C575" s="0" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B576" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="C576" s="0" t="n">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B577" s="0" t="n">
+        <v>1174</v>
+      </c>
+      <c r="C577" s="0" t="n">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B578" s="0" t="n">
+        <v>1183</v>
+      </c>
+      <c r="C578" s="0" t="n">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B579" s="0" t="n">
+        <v>1082</v>
+      </c>
+      <c r="C579" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B580" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C580" s="0" t="n">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B581" s="0" t="n">
+        <v>535</v>
+      </c>
+      <c r="C581" s="0" t="n">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B582" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="C582" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B583" s="0" t="n">
+        <v>335</v>
+      </c>
+      <c r="C583" s="0" t="n">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B584" s="0" t="n">
+        <v>1133</v>
+      </c>
+      <c r="C584" s="0" t="n">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B585" s="0" t="n">
+        <v>798</v>
+      </c>
+      <c r="C585" s="0" t="n">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B586" s="0" t="n">
+        <v>646</v>
+      </c>
+      <c r="C586" s="0" t="n">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B587" s="0" t="n">
+        <v>477</v>
+      </c>
+      <c r="C587" s="0" t="n">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B588" s="0" t="n">
+        <v>179</v>
+      </c>
+      <c r="C588" s="0" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B589" s="0" t="n">
+        <v>1194</v>
+      </c>
+      <c r="C589" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B590" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="C590" s="0" t="n">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B591" s="0" t="n">
+        <v>810</v>
+      </c>
+      <c r="C591" s="0" t="n">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B592" s="0" t="n">
+        <v>1194</v>
+      </c>
+      <c r="C592" s="0" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B593" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C593" s="0" t="n">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B594" s="0" t="n">
+        <v>945</v>
+      </c>
+      <c r="C594" s="0" t="n">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B595" s="0" t="n">
+        <v>1054</v>
+      </c>
+      <c r="C595" s="0" t="n">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B596" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="C596" s="0" t="n">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B597" s="0" t="n">
+        <v>858</v>
+      </c>
+      <c r="C597" s="0" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B598" s="0" t="n">
+        <v>570</v>
+      </c>
+      <c r="C598" s="0" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B599" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="C599" s="0" t="n">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B600" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="C600" s="0" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B601" s="0" t="n">
+        <v>889</v>
+      </c>
+      <c r="C601" s="0" t="n">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B602" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="C602" s="0" t="n">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B603" s="0" t="n">
+        <v>654</v>
+      </c>
+      <c r="C603" s="0" t="n">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B604" s="0" t="n">
+        <v>591</v>
+      </c>
+      <c r="C604" s="0" t="n">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B605" s="0" t="n">
+        <v>747</v>
+      </c>
+      <c r="C605" s="0" t="n">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B606" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="C606" s="0" t="n">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B607" s="0" t="n">
+        <v>448</v>
+      </c>
+      <c r="C607" s="0" t="n">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B608" s="0" t="n">
+        <v>1116</v>
+      </c>
+      <c r="C608" s="0" t="n">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B609" s="0" t="n">
+        <v>258</v>
+      </c>
+      <c r="C609" s="0" t="n">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B610" s="0" t="n">
+        <v>785</v>
+      </c>
+      <c r="C610" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B611" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="C611" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B612" s="0" t="n">
+        <v>884</v>
+      </c>
+      <c r="C612" s="0" t="n">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B613" s="0" t="n">
+        <v>1156</v>
+      </c>
+      <c r="C613" s="0" t="n">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B614" s="0" t="n">
+        <v>328</v>
+      </c>
+      <c r="C614" s="0" t="n">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B615" s="0" t="n">
+        <v>998</v>
+      </c>
+      <c r="C615" s="0" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B616" s="0" t="n">
+        <v>373</v>
+      </c>
+      <c r="C616" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B617" s="0" t="n">
+        <v>879</v>
+      </c>
+      <c r="C617" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B618" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="C618" s="0" t="n">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B619" s="0" t="n">
+        <v>854</v>
+      </c>
+      <c r="C619" s="0" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B620" s="0" t="n">
+        <v>457</v>
+      </c>
+      <c r="C620" s="0" t="n">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B621" s="0" t="n">
+        <v>499</v>
+      </c>
+      <c r="C621" s="0" t="n">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B622" s="0" t="n">
+        <v>552</v>
+      </c>
+      <c r="C622" s="0" t="n">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B623" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="C623" s="0" t="n">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B624" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="C624" s="0" t="n">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B625" s="0" t="n">
+        <v>1130</v>
+      </c>
+      <c r="C625" s="0" t="n">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B626" s="0" t="n">
+        <v>842</v>
+      </c>
+      <c r="C626" s="0" t="n">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B627" s="0" t="n">
+        <v>385</v>
+      </c>
+      <c r="C627" s="0" t="n">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B628" s="0" t="n">
+        <v>932</v>
+      </c>
+      <c r="C628" s="0" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B629" s="0" t="n">
+        <v>531</v>
+      </c>
+      <c r="C629" s="0" t="n">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B630" s="0" t="n">
+        <v>849</v>
+      </c>
+      <c r="C630" s="0" t="n">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B631" s="0" t="n">
+        <v>1158</v>
+      </c>
+      <c r="C631" s="0" t="n">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B632" s="0" t="n">
+        <v>688</v>
+      </c>
+      <c r="C632" s="0" t="n">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B633" s="0" t="n">
+        <v>561</v>
+      </c>
+      <c r="C633" s="0" t="n">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B634" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C634" s="0" t="n">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B635" s="0" t="n">
+        <v>956</v>
+      </c>
+      <c r="C635" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B636" s="0" t="n">
+        <v>868</v>
+      </c>
+      <c r="C636" s="0" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B637" s="0" t="n">
+        <v>1085</v>
+      </c>
+      <c r="C637" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B638" s="0" t="n">
+        <v>994</v>
+      </c>
+      <c r="C638" s="0" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B639" s="0" t="n">
+        <v>596</v>
+      </c>
+      <c r="C639" s="0" t="n">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B640" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C640" s="0" t="n">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B641" s="0" t="n">
+        <v>562</v>
+      </c>
+      <c r="C641" s="0" t="n">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B642" s="0" t="n">
+        <v>854</v>
+      </c>
+      <c r="C642" s="0" t="n">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B643" s="0" t="n">
+        <v>672</v>
+      </c>
+      <c r="C643" s="0" t="n">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B644" s="0" t="n">
+        <v>909</v>
+      </c>
+      <c r="C644" s="0" t="n">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B645" s="0" t="n">
+        <v>1065</v>
+      </c>
+      <c r="C645" s="0" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B646" s="0" t="n">
+        <v>638</v>
+      </c>
+      <c r="C646" s="0" t="n">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B647" s="0" t="n">
+        <v>488</v>
+      </c>
+      <c r="C647" s="0" t="n">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B648" s="0" t="n">
+        <v>908</v>
+      </c>
+      <c r="C648" s="0" t="n">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B649" s="0" t="n">
+        <v>918</v>
+      </c>
+      <c r="C649" s="0" t="n">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B650" s="0" t="n">
+        <v>1098</v>
+      </c>
+      <c r="C650" s="0" t="n">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B651" s="0" t="n">
+        <v>660</v>
+      </c>
+      <c r="C651" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B652" s="0" t="n">
+        <v>976</v>
+      </c>
+      <c r="C652" s="0" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B653" s="0" t="n">
+        <v>249</v>
+      </c>
+      <c r="C653" s="0" t="n">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B654" s="0" t="n">
+        <v>990</v>
+      </c>
+      <c r="C654" s="0" t="n">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B655" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C655" s="0" t="n">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B656" s="0" t="n">
+        <v>301</v>
+      </c>
+      <c r="C656" s="0" t="n">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B657" s="0" t="n">
+        <v>734</v>
+      </c>
+      <c r="C657" s="0" t="n">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B658" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="C658" s="0" t="n">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B659" s="0" t="n">
+        <v>695</v>
+      </c>
+      <c r="C659" s="0" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B660" s="0" t="n">
+        <v>662</v>
+      </c>
+      <c r="C660" s="0" t="n">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B661" s="0" t="n">
+        <v>462</v>
+      </c>
+      <c r="C661" s="0" t="n">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B662" s="0" t="n">
+        <v>976</v>
+      </c>
+      <c r="C662" s="0" t="n">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B663" s="0" t="n">
+        <v>431</v>
+      </c>
+      <c r="C663" s="0" t="n">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B664" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C664" s="0" t="n">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B665" s="0" t="n">
+        <v>603</v>
+      </c>
+      <c r="C665" s="0" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B666" s="0" t="n">
+        <v>1158</v>
+      </c>
+      <c r="C666" s="0" t="n">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B667" s="0" t="n">
+        <v>796</v>
+      </c>
+      <c r="C667" s="0" t="n">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B668" s="0" t="n">
+        <v>295</v>
+      </c>
+      <c r="C668" s="0" t="n">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B669" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="C669" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B670" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="C670" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B671" s="0" t="n">
+        <v>618</v>
+      </c>
+      <c r="C671" s="0" t="n">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B672" s="0" t="n">
+        <v>1151</v>
+      </c>
+      <c r="C672" s="0" t="n">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B673" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="C673" s="0" t="n">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B674" s="0" t="n">
+        <v>895</v>
+      </c>
+      <c r="C674" s="0" t="n">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B675" s="0" t="n">
+        <v>831</v>
+      </c>
+      <c r="C675" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B676" s="0" t="n">
+        <v>665</v>
+      </c>
+      <c r="C676" s="0" t="n">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B677" s="0" t="n">
+        <v>687</v>
+      </c>
+      <c r="C677" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B678" s="0" t="n">
+        <v>719</v>
+      </c>
+      <c r="C678" s="0" t="n">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B679" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="C679" s="0" t="n">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B680" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="C680" s="0" t="n">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B681" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C681" s="0" t="n">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B682" s="0" t="n">
+        <v>703</v>
+      </c>
+      <c r="C682" s="0" t="n">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B683" s="0" t="n">
+        <v>788</v>
+      </c>
+      <c r="C683" s="0" t="n">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B684" s="0" t="n">
+        <v>895</v>
+      </c>
+      <c r="C684" s="0" t="n">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B685" s="0" t="n">
+        <v>846</v>
+      </c>
+      <c r="C685" s="0" t="n">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B686" s="0" t="n">
+        <v>273</v>
+      </c>
+      <c r="C686" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B687" s="0" t="n">
+        <v>609</v>
+      </c>
+      <c r="C687" s="0" t="n">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B688" s="0" t="n">
+        <v>747</v>
+      </c>
+      <c r="C688" s="0" t="n">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B689" s="0" t="n">
+        <v>439</v>
+      </c>
+      <c r="C689" s="0" t="n">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B690" s="0" t="n">
+        <v>804</v>
+      </c>
+      <c r="C690" s="0" t="n">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B691" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="C691" s="0" t="n">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B692" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="C692" s="0" t="n">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B693" s="0" t="n">
+        <v>537</v>
+      </c>
+      <c r="C693" s="0" t="n">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B694" s="0" t="n">
+        <v>627</v>
+      </c>
+      <c r="C694" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B695" s="0" t="n">
+        <v>433</v>
+      </c>
+      <c r="C695" s="0" t="n">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B696" s="0" t="n">
+        <v>740</v>
+      </c>
+      <c r="C696" s="0" t="n">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B697" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="C697" s="0" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B698" s="0" t="n">
+        <v>348</v>
+      </c>
+      <c r="C698" s="0" t="n">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B699" s="0" t="n">
+        <v>1131</v>
+      </c>
+      <c r="C699" s="0" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B700" s="0" t="n">
+        <v>686</v>
+      </c>
+      <c r="C700" s="0" t="n">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B701" s="0" t="n">
+        <v>860</v>
+      </c>
+      <c r="C701" s="0" t="n">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B702" s="0" t="n">
+        <v>843</v>
+      </c>
+      <c r="C702" s="0" t="n">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B703" s="0" t="n">
+        <v>954</v>
+      </c>
+      <c r="C703" s="0" t="n">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B704" s="0" t="n">
+        <v>476</v>
+      </c>
+      <c r="C704" s="0" t="n">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B705" s="0" t="n">
+        <v>904</v>
+      </c>
+      <c r="C705" s="0" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B706" s="0" t="n">
+        <v>327</v>
+      </c>
+      <c r="C706" s="0" t="n">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B707" s="0" t="n">
+        <v>861</v>
+      </c>
+      <c r="C707" s="0" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B708" s="0" t="n">
+        <v>634</v>
+      </c>
+      <c r="C708" s="0" t="n">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B709" s="0" t="n">
+        <v>1053</v>
+      </c>
+      <c r="C709" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B710" s="0" t="n">
+        <v>282</v>
+      </c>
+      <c r="C710" s="0" t="n">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B711" s="0" t="n">
+        <v>991</v>
+      </c>
+      <c r="C711" s="0" t="n">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B712" s="0" t="n">
+        <v>425</v>
+      </c>
+      <c r="C712" s="0" t="n">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B713" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="C713" s="0" t="n">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B714" s="0" t="n">
+        <v>619</v>
+      </c>
+      <c r="C714" s="0" t="n">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B715" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="C715" s="0" t="n">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B716" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="C716" s="0" t="n">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B717" s="0" t="n">
+        <v>772</v>
+      </c>
+      <c r="C717" s="0" t="n">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B718" s="0" t="n">
+        <v>910</v>
+      </c>
+      <c r="C718" s="0" t="n">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B719" s="0" t="n">
+        <v>536</v>
+      </c>
+      <c r="C719" s="0" t="n">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B720" s="0" t="n">
+        <v>485</v>
+      </c>
+      <c r="C720" s="0" t="n">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B721" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="C721" s="0" t="n">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B722" s="0" t="n">
+        <v>662</v>
+      </c>
+      <c r="C722" s="0" t="n">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B723" s="0" t="n">
+        <v>1017</v>
+      </c>
+      <c r="C723" s="0" t="n">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B724" s="0" t="n">
+        <v>884</v>
+      </c>
+      <c r="C724" s="0" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B725" s="0" t="n">
+        <v>312</v>
+      </c>
+      <c r="C725" s="0" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B726" s="0" t="n">
+        <v>1199</v>
+      </c>
+      <c r="C726" s="0" t="n">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B727" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C727" s="0" t="n">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B728" s="0" t="n">
+        <v>378</v>
+      </c>
+      <c r="C728" s="0" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B729" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="C729" s="0" t="n">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B730" s="0" t="n">
+        <v>562</v>
+      </c>
+      <c r="C730" s="0" t="n">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B731" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="C731" s="0" t="n">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B732" s="0" t="n">
+        <v>592</v>
+      </c>
+      <c r="C732" s="0" t="n">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B733" s="0" t="n">
+        <v>674</v>
+      </c>
+      <c r="C733" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B734" s="0" t="n">
+        <v>920</v>
+      </c>
+      <c r="C734" s="0" t="n">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B735" s="0" t="n">
+        <v>1108</v>
+      </c>
+      <c r="C735" s="0" t="n">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B736" s="0" t="n">
+        <v>1079</v>
+      </c>
+      <c r="C736" s="0" t="n">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B737" s="0" t="n">
+        <v>454</v>
+      </c>
+      <c r="C737" s="0" t="n">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B738" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="C738" s="0" t="n">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B739" s="0" t="n">
+        <v>1197</v>
+      </c>
+      <c r="C739" s="0" t="n">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B740" s="0" t="n">
+        <v>710</v>
+      </c>
+      <c r="C740" s="0" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B741" s="0" t="n">
+        <v>955</v>
+      </c>
+      <c r="C741" s="0" t="n">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B742" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C742" s="0" t="n">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B743" s="0" t="n">
+        <v>1103</v>
+      </c>
+      <c r="C743" s="0" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="n">
+        <v>1</v>
+      </c>
+      <c r="B744" t="n">
+        <v>176</v>
+      </c>
+      <c r="C744" t="n">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="n">
+        <v>2</v>
+      </c>
+      <c r="B745" t="n">
+        <v>24</v>
+      </c>
+      <c r="C745" t="n">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="n">
+        <v>3</v>
+      </c>
+      <c r="B746" t="n">
+        <v>59</v>
+      </c>
+      <c r="C746" t="n">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="n">
+        <v>4</v>
+      </c>
+      <c r="B747" t="n">
+        <v>1150</v>
+      </c>
+      <c r="C747" t="n">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="n">
+        <v>5</v>
+      </c>
+      <c r="B748" t="n">
+        <v>779</v>
+      </c>
+      <c r="C748" t="n">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="n">
+        <v>6</v>
+      </c>
+      <c r="B749" t="n">
+        <v>184</v>
+      </c>
+      <c r="C749" t="n">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="n">
+        <v>7</v>
+      </c>
+      <c r="B750" t="n">
+        <v>976</v>
+      </c>
+      <c r="C750" t="n">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="n">
+        <v>8</v>
+      </c>
+      <c r="B751" t="n">
+        <v>496</v>
+      </c>
+      <c r="C751" t="n">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="n">
+        <v>9</v>
+      </c>
+      <c r="B752" t="n">
+        <v>757</v>
+      </c>
+      <c r="C752" t="n">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="n">
+        <v>10</v>
+      </c>
+      <c r="B753" t="n">
+        <v>561</v>
+      </c>
+      <c r="C753" t="n">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="n">
+        <v>11</v>
+      </c>
+      <c r="B754" t="n">
+        <v>788</v>
+      </c>
+      <c r="C754" t="n">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="n">
+        <v>12</v>
+      </c>
+      <c r="B755" t="n">
+        <v>672</v>
+      </c>
+      <c r="C755" t="n">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="n">
+        <v>13</v>
+      </c>
+      <c r="B756" t="n">
+        <v>441</v>
+      </c>
+      <c r="C756" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="n">
+        <v>14</v>
+      </c>
+      <c r="B757" t="n">
+        <v>1072</v>
+      </c>
+      <c r="C757" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="n">
+        <v>15</v>
+      </c>
+      <c r="B758" t="n">
+        <v>857</v>
+      </c>
+      <c r="C758" t="n">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="n">
+        <v>16</v>
+      </c>
+      <c r="B759" t="n">
+        <v>654</v>
+      </c>
+      <c r="C759" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="n">
+        <v>17</v>
+      </c>
+      <c r="B760" t="n">
+        <v>447</v>
+      </c>
+      <c r="C760" t="n">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="n">
+        <v>18</v>
+      </c>
+      <c r="B761" t="n">
+        <v>1052</v>
+      </c>
+      <c r="C761" t="n">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="n">
+        <v>19</v>
+      </c>
+      <c r="B762" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C762" t="n">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="n">
+        <v>20</v>
+      </c>
+      <c r="B763" t="n">
+        <v>207</v>
+      </c>
+      <c r="C763" t="n">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="n">
+        <v>21</v>
+      </c>
+      <c r="B764" t="n">
+        <v>525</v>
+      </c>
+      <c r="C764" t="n">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="n">
+        <v>22</v>
+      </c>
+      <c r="B765" t="n">
+        <v>585</v>
+      </c>
+      <c r="C765" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="n">
+        <v>23</v>
+      </c>
+      <c r="B766" t="n">
+        <v>939</v>
+      </c>
+      <c r="C766" t="n">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="n">
+        <v>24</v>
+      </c>
+      <c r="B767" t="n">
+        <v>714</v>
+      </c>
+      <c r="C767" t="n">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="n">
+        <v>25</v>
+      </c>
+      <c r="B768" t="n">
+        <v>305</v>
+      </c>
+      <c r="C768" t="n">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="n">
+        <v>26</v>
+      </c>
+      <c r="B769" t="n">
+        <v>909</v>
+      </c>
+      <c r="C769" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="n">
+        <v>27</v>
+      </c>
+      <c r="B770" t="n">
+        <v>1020</v>
+      </c>
+      <c r="C770" t="n">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="n">
+        <v>28</v>
+      </c>
+      <c r="B771" t="n">
+        <v>937</v>
+      </c>
+      <c r="C771" t="n">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="n">
+        <v>29</v>
+      </c>
+      <c r="B772" t="n">
+        <v>747</v>
+      </c>
+      <c r="C772" t="n">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="n">
+        <v>30</v>
+      </c>
+      <c r="B773" t="n">
+        <v>188</v>
+      </c>
+      <c r="C773" t="n">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="n">
+        <v>31</v>
+      </c>
+      <c r="B774" t="n">
+        <v>17</v>
+      </c>
+      <c r="C774" t="n">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="n">
+        <v>32</v>
+      </c>
+      <c r="B775" t="n">
+        <v>747</v>
+      </c>
+      <c r="C775" t="n">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="n">
+        <v>33</v>
+      </c>
+      <c r="B776" t="n">
+        <v>460</v>
+      </c>
+      <c r="C776" t="n">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="n">
+        <v>34</v>
+      </c>
+      <c r="B777" t="n">
+        <v>315</v>
+      </c>
+      <c r="C777" t="n">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="n">
+        <v>35</v>
+      </c>
+      <c r="B778" t="n">
+        <v>393</v>
+      </c>
+      <c r="C778" t="n">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="n">
+        <v>36</v>
+      </c>
+      <c r="B779" t="n">
+        <v>832</v>
+      </c>
+      <c r="C779" t="n">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="n">
+        <v>37</v>
+      </c>
+      <c r="B780" t="n">
+        <v>765</v>
+      </c>
+      <c r="C780" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="n">
+        <v>38</v>
+      </c>
+      <c r="B781" t="n">
+        <v>1055</v>
+      </c>
+      <c r="C781" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="n">
+        <v>39</v>
+      </c>
+      <c r="B782" t="n">
+        <v>200</v>
+      </c>
+      <c r="C782" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="n">
+        <v>40</v>
+      </c>
+      <c r="B783" t="n">
+        <v>549</v>
+      </c>
+      <c r="C783" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="n">
+        <v>41</v>
+      </c>
+      <c r="B784" t="n">
+        <v>115</v>
+      </c>
+      <c r="C784" t="n">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="n">
+        <v>42</v>
+      </c>
+      <c r="B785" t="n">
+        <v>880</v>
+      </c>
+      <c r="C785" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="n">
+        <v>43</v>
+      </c>
+      <c r="B786" t="n">
+        <v>918</v>
+      </c>
+      <c r="C786" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="n">
+        <v>44</v>
+      </c>
+      <c r="B787" t="n">
+        <v>148</v>
+      </c>
+      <c r="C787" t="n">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="n">
+        <v>45</v>
+      </c>
+      <c r="B788" t="n">
+        <v>436</v>
+      </c>
+      <c r="C788" t="n">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="n">
+        <v>46</v>
+      </c>
+      <c r="B789" t="n">
+        <v>261</v>
+      </c>
+      <c r="C789" t="n">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="n">
+        <v>47</v>
+      </c>
+      <c r="B790" t="n">
+        <v>441</v>
+      </c>
+      <c r="C790" t="n">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="n">
+        <v>48</v>
+      </c>
+      <c r="B791" t="n">
+        <v>430</v>
+      </c>
+      <c r="C791" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="n">
+        <v>49</v>
+      </c>
+      <c r="B792" t="n">
+        <v>333</v>
+      </c>
+      <c r="C792" t="n">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="n">
+        <v>50</v>
+      </c>
+      <c r="B793" t="n">
+        <v>106</v>
+      </c>
+      <c r="C793" t="n">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifications de l'interface utilisateur plus besoin de passer par le terminal
</commit_message>
<xml_diff>
--- a/ListPoint.xlsx
+++ b/ListPoint.xlsx
@@ -262,7 +262,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C793"/>
+  <dimension ref="A1:C956"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
@@ -8444,553 +8444,2346 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" t="n">
+      <c r="A744" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B744" t="n">
+      <c r="B744" s="0" t="n">
         <v>176</v>
       </c>
-      <c r="C744" t="n">
+      <c r="C744" s="0" t="n">
         <v>595</v>
       </c>
     </row>
     <row r="745">
-      <c r="A745" t="n">
+      <c r="A745" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B745" t="n">
+      <c r="B745" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="C745" t="n">
+      <c r="C745" s="0" t="n">
         <v>380</v>
       </c>
     </row>
     <row r="746">
-      <c r="A746" t="n">
+      <c r="A746" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B746" t="n">
+      <c r="B746" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="C746" t="n">
+      <c r="C746" s="0" t="n">
         <v>188</v>
       </c>
     </row>
     <row r="747">
-      <c r="A747" t="n">
+      <c r="A747" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B747" t="n">
+      <c r="B747" s="0" t="n">
         <v>1150</v>
       </c>
-      <c r="C747" t="n">
+      <c r="C747" s="0" t="n">
         <v>715</v>
       </c>
     </row>
     <row r="748">
-      <c r="A748" t="n">
+      <c r="A748" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B748" t="n">
+      <c r="B748" s="0" t="n">
         <v>779</v>
       </c>
-      <c r="C748" t="n">
+      <c r="C748" s="0" t="n">
         <v>163</v>
       </c>
     </row>
     <row r="749">
-      <c r="A749" t="n">
+      <c r="A749" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B749" t="n">
+      <c r="B749" s="0" t="n">
         <v>184</v>
       </c>
-      <c r="C749" t="n">
+      <c r="C749" s="0" t="n">
         <v>649</v>
       </c>
     </row>
     <row r="750">
-      <c r="A750" t="n">
+      <c r="A750" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B750" t="n">
+      <c r="B750" s="0" t="n">
         <v>976</v>
       </c>
-      <c r="C750" t="n">
+      <c r="C750" s="0" t="n">
         <v>702</v>
       </c>
     </row>
     <row r="751">
-      <c r="A751" t="n">
+      <c r="A751" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B751" t="n">
+      <c r="B751" s="0" t="n">
         <v>496</v>
       </c>
-      <c r="C751" t="n">
+      <c r="C751" s="0" t="n">
         <v>676</v>
       </c>
     </row>
     <row r="752">
-      <c r="A752" t="n">
+      <c r="A752" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B752" t="n">
+      <c r="B752" s="0" t="n">
         <v>757</v>
       </c>
-      <c r="C752" t="n">
+      <c r="C752" s="0" t="n">
         <v>895</v>
       </c>
     </row>
     <row r="753">
-      <c r="A753" t="n">
+      <c r="A753" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B753" t="n">
+      <c r="B753" s="0" t="n">
         <v>561</v>
       </c>
-      <c r="C753" t="n">
+      <c r="C753" s="0" t="n">
         <v>247</v>
       </c>
     </row>
     <row r="754">
-      <c r="A754" t="n">
+      <c r="A754" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B754" t="n">
+      <c r="B754" s="0" t="n">
         <v>788</v>
       </c>
-      <c r="C754" t="n">
+      <c r="C754" s="0" t="n">
         <v>677</v>
       </c>
     </row>
     <row r="755">
-      <c r="A755" t="n">
+      <c r="A755" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B755" t="n">
+      <c r="B755" s="0" t="n">
         <v>672</v>
       </c>
-      <c r="C755" t="n">
+      <c r="C755" s="0" t="n">
         <v>573</v>
       </c>
     </row>
     <row r="756">
-      <c r="A756" t="n">
+      <c r="A756" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B756" t="n">
+      <c r="B756" s="0" t="n">
         <v>441</v>
       </c>
-      <c r="C756" t="n">
+      <c r="C756" s="0" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="757">
-      <c r="A757" t="n">
+      <c r="A757" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B757" t="n">
+      <c r="B757" s="0" t="n">
         <v>1072</v>
       </c>
-      <c r="C757" t="n">
+      <c r="C757" s="0" t="n">
         <v>138</v>
       </c>
     </row>
     <row r="758">
-      <c r="A758" t="n">
+      <c r="A758" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B758" t="n">
+      <c r="B758" s="0" t="n">
         <v>857</v>
       </c>
-      <c r="C758" t="n">
+      <c r="C758" s="0" t="n">
         <v>390</v>
       </c>
     </row>
     <row r="759">
-      <c r="A759" t="n">
+      <c r="A759" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B759" t="n">
+      <c r="B759" s="0" t="n">
         <v>654</v>
       </c>
-      <c r="C759" t="n">
+      <c r="C759" s="0" t="n">
         <v>303</v>
       </c>
     </row>
     <row r="760">
-      <c r="A760" t="n">
+      <c r="A760" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B760" t="n">
+      <c r="B760" s="0" t="n">
         <v>447</v>
       </c>
-      <c r="C760" t="n">
+      <c r="C760" s="0" t="n">
         <v>747</v>
       </c>
     </row>
     <row r="761">
-      <c r="A761" t="n">
+      <c r="A761" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B761" t="n">
+      <c r="B761" s="0" t="n">
         <v>1052</v>
       </c>
-      <c r="C761" t="n">
+      <c r="C761" s="0" t="n">
         <v>407</v>
       </c>
     </row>
     <row r="762">
-      <c r="A762" t="n">
+      <c r="A762" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B762" t="n">
+      <c r="B762" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="C762" t="n">
+      <c r="C762" s="0" t="n">
         <v>517</v>
       </c>
     </row>
     <row r="763">
-      <c r="A763" t="n">
+      <c r="A763" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B763" t="n">
+      <c r="B763" s="0" t="n">
         <v>207</v>
       </c>
-      <c r="C763" t="n">
+      <c r="C763" s="0" t="n">
         <v>783</v>
       </c>
     </row>
     <row r="764">
-      <c r="A764" t="n">
+      <c r="A764" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B764" t="n">
+      <c r="B764" s="0" t="n">
         <v>525</v>
       </c>
-      <c r="C764" t="n">
+      <c r="C764" s="0" t="n">
         <v>286</v>
       </c>
     </row>
     <row r="765">
-      <c r="A765" t="n">
+      <c r="A765" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B765" t="n">
+      <c r="B765" s="0" t="n">
         <v>585</v>
       </c>
-      <c r="C765" t="n">
+      <c r="C765" s="0" t="n">
         <v>680</v>
       </c>
     </row>
     <row r="766">
-      <c r="A766" t="n">
+      <c r="A766" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B766" t="n">
+      <c r="B766" s="0" t="n">
         <v>939</v>
       </c>
-      <c r="C766" t="n">
+      <c r="C766" s="0" t="n">
         <v>847</v>
       </c>
     </row>
     <row r="767">
-      <c r="A767" t="n">
+      <c r="A767" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B767" t="n">
+      <c r="B767" s="0" t="n">
         <v>714</v>
       </c>
-      <c r="C767" t="n">
+      <c r="C767" s="0" t="n">
         <v>444</v>
       </c>
     </row>
     <row r="768">
-      <c r="A768" t="n">
+      <c r="A768" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B768" t="n">
+      <c r="B768" s="0" t="n">
         <v>305</v>
       </c>
-      <c r="C768" t="n">
+      <c r="C768" s="0" t="n">
         <v>520</v>
       </c>
     </row>
     <row r="769">
-      <c r="A769" t="n">
+      <c r="A769" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B769" t="n">
+      <c r="B769" s="0" t="n">
         <v>909</v>
       </c>
-      <c r="C769" t="n">
+      <c r="C769" s="0" t="n">
         <v>485</v>
       </c>
     </row>
     <row r="770">
-      <c r="A770" t="n">
+      <c r="A770" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B770" t="n">
+      <c r="B770" s="0" t="n">
         <v>1020</v>
       </c>
-      <c r="C770" t="n">
+      <c r="C770" s="0" t="n">
         <v>729</v>
       </c>
     </row>
     <row r="771">
-      <c r="A771" t="n">
+      <c r="A771" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B771" t="n">
+      <c r="B771" s="0" t="n">
         <v>937</v>
       </c>
-      <c r="C771" t="n">
+      <c r="C771" s="0" t="n">
         <v>382</v>
       </c>
     </row>
     <row r="772">
-      <c r="A772" t="n">
+      <c r="A772" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B772" t="n">
+      <c r="B772" s="0" t="n">
         <v>747</v>
       </c>
-      <c r="C772" t="n">
+      <c r="C772" s="0" t="n">
         <v>663</v>
       </c>
     </row>
     <row r="773">
-      <c r="A773" t="n">
+      <c r="A773" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B773" t="n">
+      <c r="B773" s="0" t="n">
         <v>188</v>
       </c>
-      <c r="C773" t="n">
+      <c r="C773" s="0" t="n">
         <v>378</v>
       </c>
     </row>
     <row r="774">
-      <c r="A774" t="n">
+      <c r="A774" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B774" t="n">
+      <c r="B774" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="C774" t="n">
+      <c r="C774" s="0" t="n">
         <v>219</v>
       </c>
     </row>
     <row r="775">
-      <c r="A775" t="n">
+      <c r="A775" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B775" t="n">
+      <c r="B775" s="0" t="n">
         <v>747</v>
       </c>
-      <c r="C775" t="n">
+      <c r="C775" s="0" t="n">
         <v>460</v>
       </c>
     </row>
     <row r="776">
-      <c r="A776" t="n">
+      <c r="A776" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B776" t="n">
+      <c r="B776" s="0" t="n">
         <v>460</v>
       </c>
-      <c r="C776" t="n">
+      <c r="C776" s="0" t="n">
         <v>196</v>
       </c>
     </row>
     <row r="777">
-      <c r="A777" t="n">
+      <c r="A777" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B777" t="n">
+      <c r="B777" s="0" t="n">
         <v>315</v>
       </c>
-      <c r="C777" t="n">
+      <c r="C777" s="0" t="n">
         <v>426</v>
       </c>
     </row>
     <row r="778">
-      <c r="A778" t="n">
+      <c r="A778" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B778" t="n">
+      <c r="B778" s="0" t="n">
         <v>393</v>
       </c>
-      <c r="C778" t="n">
+      <c r="C778" s="0" t="n">
         <v>333</v>
       </c>
     </row>
     <row r="779">
-      <c r="A779" t="n">
+      <c r="A779" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B779" t="n">
+      <c r="B779" s="0" t="n">
         <v>832</v>
       </c>
-      <c r="C779" t="n">
+      <c r="C779" s="0" t="n">
         <v>847</v>
       </c>
     </row>
     <row r="780">
-      <c r="A780" t="n">
+      <c r="A780" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B780" t="n">
+      <c r="B780" s="0" t="n">
         <v>765</v>
       </c>
-      <c r="C780" t="n">
+      <c r="C780" s="0" t="n">
         <v>260</v>
       </c>
     </row>
     <row r="781">
-      <c r="A781" t="n">
+      <c r="A781" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B781" t="n">
+      <c r="B781" s="0" t="n">
         <v>1055</v>
       </c>
-      <c r="C781" t="n">
+      <c r="C781" s="0" t="n">
         <v>115</v>
       </c>
     </row>
     <row r="782">
-      <c r="A782" t="n">
+      <c r="A782" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B782" t="n">
+      <c r="B782" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="C782" t="n">
+      <c r="C782" s="0" t="n">
         <v>210</v>
       </c>
     </row>
     <row r="783">
-      <c r="A783" t="n">
+      <c r="A783" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B783" t="n">
+      <c r="B783" s="0" t="n">
         <v>549</v>
       </c>
-      <c r="C783" t="n">
+      <c r="C783" s="0" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="784">
-      <c r="A784" t="n">
+      <c r="A784" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B784" t="n">
+      <c r="B784" s="0" t="n">
         <v>115</v>
       </c>
-      <c r="C784" t="n">
+      <c r="C784" s="0" t="n">
         <v>473</v>
       </c>
     </row>
     <row r="785">
-      <c r="A785" t="n">
+      <c r="A785" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B785" t="n">
+      <c r="B785" s="0" t="n">
         <v>880</v>
       </c>
-      <c r="C785" t="n">
+      <c r="C785" s="0" t="n">
         <v>800</v>
       </c>
     </row>
     <row r="786">
-      <c r="A786" t="n">
+      <c r="A786" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B786" t="n">
+      <c r="B786" s="0" t="n">
         <v>918</v>
       </c>
-      <c r="C786" t="n">
+      <c r="C786" s="0" t="n">
         <v>129</v>
       </c>
     </row>
     <row r="787">
-      <c r="A787" t="n">
+      <c r="A787" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B787" t="n">
+      <c r="B787" s="0" t="n">
         <v>148</v>
       </c>
-      <c r="C787" t="n">
+      <c r="C787" s="0" t="n">
         <v>810</v>
       </c>
     </row>
     <row r="788">
-      <c r="A788" t="n">
+      <c r="A788" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B788" t="n">
+      <c r="B788" s="0" t="n">
         <v>436</v>
       </c>
-      <c r="C788" t="n">
+      <c r="C788" s="0" t="n">
         <v>282</v>
       </c>
     </row>
     <row r="789">
-      <c r="A789" t="n">
+      <c r="A789" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B789" t="n">
+      <c r="B789" s="0" t="n">
         <v>261</v>
       </c>
-      <c r="C789" t="n">
+      <c r="C789" s="0" t="n">
         <v>138</v>
       </c>
     </row>
     <row r="790">
-      <c r="A790" t="n">
+      <c r="A790" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B790" t="n">
+      <c r="B790" s="0" t="n">
         <v>441</v>
       </c>
-      <c r="C790" t="n">
+      <c r="C790" s="0" t="n">
         <v>221</v>
       </c>
     </row>
     <row r="791">
-      <c r="A791" t="n">
+      <c r="A791" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B791" t="n">
+      <c r="B791" s="0" t="n">
         <v>430</v>
       </c>
-      <c r="C791" t="n">
+      <c r="C791" s="0" t="n">
         <v>178</v>
       </c>
     </row>
     <row r="792">
-      <c r="A792" t="n">
+      <c r="A792" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B792" t="n">
+      <c r="B792" s="0" t="n">
         <v>333</v>
       </c>
-      <c r="C792" t="n">
+      <c r="C792" s="0" t="n">
         <v>491</v>
       </c>
     </row>
     <row r="793">
-      <c r="A793" t="n">
+      <c r="A793" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B793" t="n">
+      <c r="B793" s="0" t="n">
         <v>106</v>
       </c>
-      <c r="C793" t="n">
+      <c r="C793" s="0" t="n">
         <v>251</v>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B794" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C794" s="0" t="n">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B795" s="0" t="n">
+        <v>453</v>
+      </c>
+      <c r="C795" s="0" t="n">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B796" s="0" t="n">
+        <v>872</v>
+      </c>
+      <c r="C796" s="0" t="n">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B797" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="C797" s="0" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B798" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="C798" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B799" s="0" t="n">
+        <v>728</v>
+      </c>
+      <c r="C799" s="0" t="n">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B800" s="0" t="n">
+        <v>458</v>
+      </c>
+      <c r="C800" s="0" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B801" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="C801" s="0" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B802" s="0" t="n">
+        <v>496</v>
+      </c>
+      <c r="C802" s="0" t="n">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B803" s="0" t="n">
+        <v>291</v>
+      </c>
+      <c r="C803" s="0" t="n">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B804" s="0" t="n">
+        <v>1132</v>
+      </c>
+      <c r="C804" s="0" t="n">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B805" s="0" t="n">
+        <v>970</v>
+      </c>
+      <c r="C805" s="0" t="n">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B806" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="C806" s="0" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B807" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="C807" s="0" t="n">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B808" s="0" t="n">
+        <v>998</v>
+      </c>
+      <c r="C808" s="0" t="n">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B809" s="0" t="n">
+        <v>569</v>
+      </c>
+      <c r="C809" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B810" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="C810" s="0" t="n">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B811" s="0" t="n">
+        <v>1006</v>
+      </c>
+      <c r="C811" s="0" t="n">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B812" s="0" t="n">
+        <v>441</v>
+      </c>
+      <c r="C812" s="0" t="n">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B813" s="0" t="n">
+        <v>504</v>
+      </c>
+      <c r="C813" s="0" t="n">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B814" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C814" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B815" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="C815" s="0" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B816" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="C816" s="0" t="n">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B817" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C817" s="0" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B818" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C818" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B819" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="C819" s="0" t="n">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B820" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C820" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B821" s="0" t="n">
+        <v>840</v>
+      </c>
+      <c r="C821" s="0" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B822" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C822" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B823" s="0" t="n">
+        <v>995</v>
+      </c>
+      <c r="C823" s="0" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B824" s="0" t="n">
+        <v>809</v>
+      </c>
+      <c r="C824" s="0" t="n">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B825" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="C825" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B826" s="0" t="n">
+        <v>1172</v>
+      </c>
+      <c r="C826" s="0" t="n">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B827" s="0" t="n">
+        <v>255</v>
+      </c>
+      <c r="C827" s="0" t="n">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B828" s="0" t="n">
+        <v>630</v>
+      </c>
+      <c r="C828" s="0" t="n">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B829" s="0" t="n">
+        <v>343</v>
+      </c>
+      <c r="C829" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B830" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="C830" s="0" t="n">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B831" s="0" t="n">
+        <v>1062</v>
+      </c>
+      <c r="C831" s="0" t="n">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B832" s="0" t="n">
+        <v>625</v>
+      </c>
+      <c r="C832" s="0" t="n">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B833" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C833" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B834" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="C834" s="0" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B835" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="C835" s="0" t="n">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B836" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C836" s="0" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B837" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C837" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B838" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="C838" s="0" t="n">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B839" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C839" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B840" s="0" t="n">
+        <v>840</v>
+      </c>
+      <c r="C840" s="0" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B841" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C841" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B842" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C842" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B843" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="C843" s="0" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B844" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="C844" s="0" t="n">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B845" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C845" s="0" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B846" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C846" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B847" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="C847" s="0" t="n">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B848" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C848" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B849" s="0" t="n">
+        <v>840</v>
+      </c>
+      <c r="C849" s="0" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B850" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C850" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B851" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C851" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B852" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="C852" s="0" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B853" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="C853" s="0" t="n">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B854" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C854" s="0" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B855" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C855" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B856" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="C856" s="0" t="n">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B857" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C857" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B858" s="0" t="n">
+        <v>840</v>
+      </c>
+      <c r="C858" s="0" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B859" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C859" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B860" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C860" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B861" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="C861" s="0" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B862" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="C862" s="0" t="n">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B863" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C863" s="0" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="B864" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C864" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B865" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="C865" s="0" t="n">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="B866" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C866" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B867" s="0" t="n">
+        <v>840</v>
+      </c>
+      <c r="C867" s="0" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B868" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C868" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="B869" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="C869" s="0" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B870" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="C870" s="0" t="n">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B871" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C871" s="0" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B872" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C872" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="B873" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="C873" s="0" t="n">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B874" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C874" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B875" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="C875" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="B876" s="0" t="n">
+        <v>310</v>
+      </c>
+      <c r="C876" s="0" t="n">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B877" s="0" t="n">
+        <v>222</v>
+      </c>
+      <c r="C877" s="0" t="n">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="B878" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C878" s="0" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B879" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C879" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="B880" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="C880" s="0" t="n">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B881" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C881" s="0" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="B882" s="0" t="n">
+        <v>840</v>
+      </c>
+      <c r="C882" s="0" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B883" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C883" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B884" s="0" t="n">
+        <v>840</v>
+      </c>
+      <c r="C884" s="0" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B885" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C885" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="B886" s="0" t="n">
+        <v>380</v>
+      </c>
+      <c r="C886" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B887" s="0" t="n">
+        <v>1082</v>
+      </c>
+      <c r="C887" s="0" t="n">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="B888" s="0" t="n">
+        <v>166</v>
+      </c>
+      <c r="C888" s="0" t="n">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B889" s="0" t="n">
+        <v>939</v>
+      </c>
+      <c r="C889" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="B890" s="0" t="n">
+        <v>231</v>
+      </c>
+      <c r="C890" s="0" t="n">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B891" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="C891" s="0" t="n">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="B892" s="0" t="n">
+        <v>1091</v>
+      </c>
+      <c r="C892" s="0" t="n">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B893" s="0" t="n">
+        <v>823</v>
+      </c>
+      <c r="C893" s="0" t="n">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="B894" s="0" t="n">
+        <v>219</v>
+      </c>
+      <c r="C894" s="0" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B895" s="0" t="n">
+        <v>680</v>
+      </c>
+      <c r="C895" s="0" t="n">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="B896" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="C896" s="0" t="n">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B897" s="0" t="n">
+        <v>985</v>
+      </c>
+      <c r="C897" s="0" t="n">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="B898" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="C898" s="0" t="n">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="B899" s="0" t="n">
+        <v>507</v>
+      </c>
+      <c r="C899" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="B900" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C900" s="0" t="n">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B901" s="0" t="n">
+        <v>1028</v>
+      </c>
+      <c r="C901" s="0" t="n">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="B902" s="0" t="n">
+        <v>717</v>
+      </c>
+      <c r="C902" s="0" t="n">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B903" s="0" t="n">
+        <v>277</v>
+      </c>
+      <c r="C903" s="0" t="n">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="B904" s="0" t="n">
+        <v>759</v>
+      </c>
+      <c r="C904" s="0" t="n">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B905" s="0" t="n">
+        <v>759</v>
+      </c>
+      <c r="C905" s="0" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="B906" s="0" t="n">
+        <v>382</v>
+      </c>
+      <c r="C906" s="0" t="n">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B907" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="C907" s="0" t="n">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B908" s="0" t="n">
+        <v>597</v>
+      </c>
+      <c r="C908" s="0" t="n">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B909" s="0" t="n">
+        <v>1179</v>
+      </c>
+      <c r="C909" s="0" t="n">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B910" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="C910" s="0" t="n">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B911" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="C911" s="0" t="n">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B912" s="0" t="n">
+        <v>401</v>
+      </c>
+      <c r="C912" s="0" t="n">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B913" s="0" t="n">
+        <v>1036</v>
+      </c>
+      <c r="C913" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B914" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="C914" s="0" t="n">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B915" s="0" t="n">
+        <v>748</v>
+      </c>
+      <c r="C915" s="0" t="n">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B916" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C916" s="0" t="n">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B917" s="0" t="n">
+        <v>475</v>
+      </c>
+      <c r="C917" s="0" t="n">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B918" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C918" s="0" t="n">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B919" s="0" t="n">
+        <v>1022</v>
+      </c>
+      <c r="C919" s="0" t="n">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B920" s="0" t="n">
+        <v>382</v>
+      </c>
+      <c r="C920" s="0" t="n">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B921" s="0" t="n">
+        <v>1167</v>
+      </c>
+      <c r="C921" s="0" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B922" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="C922" s="0" t="n">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B923" s="0" t="n">
+        <v>588</v>
+      </c>
+      <c r="C923" s="0" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B924" s="0" t="n">
+        <v>862</v>
+      </c>
+      <c r="C924" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B925" s="0" t="n">
+        <v>1086</v>
+      </c>
+      <c r="C925" s="0" t="n">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B926" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="C926" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B927" s="0" t="n">
+        <v>897</v>
+      </c>
+      <c r="C927" s="0" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B928" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="C928" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B929" s="0" t="n">
+        <v>516</v>
+      </c>
+      <c r="C929" s="0" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B930" s="0" t="n">
+        <v>727</v>
+      </c>
+      <c r="C930" s="0" t="n">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B931" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="C931" s="0" t="n">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B932" s="0" t="n">
+        <v>621</v>
+      </c>
+      <c r="C932" s="0" t="n">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B933" s="0" t="n">
+        <v>1116</v>
+      </c>
+      <c r="C933" s="0" t="n">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B934" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="C934" s="0" t="n">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B935" s="0" t="n">
+        <v>822</v>
+      </c>
+      <c r="C935" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B936" s="0" t="n">
+        <v>169</v>
+      </c>
+      <c r="C936" s="0" t="n">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B937" s="0" t="n">
+        <v>562</v>
+      </c>
+      <c r="C937" s="0" t="n">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B938" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="C938" s="0" t="n">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B939" s="0" t="n">
+        <v>378</v>
+      </c>
+      <c r="C939" s="0" t="n">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B940" s="0" t="n">
+        <v>609</v>
+      </c>
+      <c r="C940" s="0" t="n">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B941" s="0" t="n">
+        <v>880</v>
+      </c>
+      <c r="C941" s="0" t="n">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B942" s="0" t="n">
+        <v>874</v>
+      </c>
+      <c r="C942" s="0" t="n">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B943" s="0" t="n">
+        <v>894</v>
+      </c>
+      <c r="C943" s="0" t="n">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B944" s="0" t="n">
+        <v>846</v>
+      </c>
+      <c r="C944" s="0" t="n">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B945" s="0" t="n">
+        <v>406</v>
+      </c>
+      <c r="C945" s="0" t="n">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B946" s="0" t="n">
+        <v>462</v>
+      </c>
+      <c r="C946" s="0" t="n">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="n">
+        <v>1</v>
+      </c>
+      <c r="B947" t="n">
+        <v>124</v>
+      </c>
+      <c r="C947" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="n">
+        <v>2</v>
+      </c>
+      <c r="B948" t="n">
+        <v>1155</v>
+      </c>
+      <c r="C948" t="n">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="n">
+        <v>3</v>
+      </c>
+      <c r="B949" t="n">
+        <v>400</v>
+      </c>
+      <c r="C949" t="n">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="n">
+        <v>4</v>
+      </c>
+      <c r="B950" t="n">
+        <v>709</v>
+      </c>
+      <c r="C950" t="n">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="n">
+        <v>5</v>
+      </c>
+      <c r="B951" t="n">
+        <v>1055</v>
+      </c>
+      <c r="C951" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="n">
+        <v>6</v>
+      </c>
+      <c r="B952" t="n">
+        <v>587</v>
+      </c>
+      <c r="C952" t="n">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="n">
+        <v>7</v>
+      </c>
+      <c r="B953" t="n">
+        <v>940</v>
+      </c>
+      <c r="C953" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="n">
+        <v>8</v>
+      </c>
+      <c r="B954" t="n">
+        <v>142</v>
+      </c>
+      <c r="C954" t="n">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="n">
+        <v>9</v>
+      </c>
+      <c r="B955" t="n">
+        <v>440</v>
+      </c>
+      <c r="C955" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="n">
+        <v>10</v>
+      </c>
+      <c r="B956" t="n">
+        <v>849</v>
+      </c>
+      <c r="C956" t="n">
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>